<commit_message>
ültimas modificaciones para entrega sw2 21-02-2020
</commit_message>
<xml_diff>
--- a/Documentos/02 Requisitos/005 ESP_DET_WRRS_ Modulo de ingreso al sistema_.xlsx
+++ b/Documentos/02 Requisitos/005 ESP_DET_WRRS_ Modulo de ingreso al sistema_.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Universidad\10 Semestre\Proyecto SW1\ProyectoLaVozDelRioSuarez\Documentos\02 Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duvan\Documents\Universidad\10 Semestre\Proyecto SW1\ProyectoLaVozDelRioSuarez\Documentos\02 Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Orden de navegación</t>
   </si>
@@ -60,15 +60,6 @@
     <t>Tipo de campo</t>
   </si>
   <si>
-    <t>Número máximo de dígitos</t>
-  </si>
-  <si>
-    <t>Dígitos numéricos enteros</t>
-  </si>
-  <si>
-    <t>Dígitos numéricos decimales</t>
-  </si>
-  <si>
     <t>Input text</t>
   </si>
   <si>
@@ -93,79 +84,67 @@
     <t>Los campos de usuario y contraseña deben ser correctos</t>
   </si>
   <si>
-    <t>El usuario será redireccionado a una ventana en donde se le indicarán los pasos que debe seguir para restablecer la contraseña</t>
-  </si>
-  <si>
-    <t>Restablecer mi contraseña</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
     <t>El usuario ya debe estar registrado en el sistema.</t>
   </si>
   <si>
-    <t>Correo de usuario</t>
-  </si>
-  <si>
     <t>Input password</t>
   </si>
   <si>
     <t>Campo para el ingreso del correo electrónico del usuario</t>
   </si>
   <si>
-    <t>Correo o contraseña incorrectos</t>
-  </si>
-  <si>
-    <t>Correo no encontrado en el sistema</t>
-  </si>
-  <si>
     <t>Al ser presionado el sistema valida que los datos ingresados en los campos de Correo electrónico y contraseña sean correctos; si ese es el caso, el usuario ingresa a la apliación respectiva al tipo de usuario. En caso contrario se debe mostrar el error con el mensaje que informe el tipo de este.</t>
   </si>
   <si>
     <t>El campo de correo electrónico y contraseña deben contener texto</t>
   </si>
   <si>
-    <t>Corrreo electrónico incorrecto.</t>
-  </si>
-  <si>
-    <t>Correo electrónico o contraseña incorrectos</t>
-  </si>
-  <si>
-    <t>El correo o la contraseña son incorrectos. Intentelo nuevamente</t>
-  </si>
-  <si>
     <t>Campo para el ingreso de contraseña correspondinete al correo ingresado.</t>
   </si>
   <si>
     <t>La contraseña debe coincidir con la asociada al correo electrónico ingresado anteriormente</t>
   </si>
   <si>
-    <t xml:space="preserve">Contraseña </t>
-  </si>
-  <si>
     <t>Puede recibir caracteres alfanuméricos y especiales</t>
   </si>
   <si>
     <t>Si</t>
   </si>
   <si>
-    <t>Iniciar</t>
-  </si>
-  <si>
     <t>Iniciar sesión</t>
   </si>
   <si>
-    <t>Olvide mi contraseña</t>
-  </si>
-  <si>
     <t>No hay validaciones</t>
   </si>
   <si>
-    <t>Registrarme</t>
-  </si>
-  <si>
     <t>Al ser presionado mostrará una ventana en la cual el usuario podrá realizar el registro en el sistema</t>
+  </si>
+  <si>
+    <t>Registrarse</t>
+  </si>
+  <si>
+    <t>Registrarse en el sistema</t>
+  </si>
+  <si>
+    <t>Ingresar</t>
+  </si>
+  <si>
+    <t>Número máximo de caracteres</t>
+  </si>
+  <si>
+    <t>Número mínimo de caracteres</t>
+  </si>
+  <si>
+    <t>1. Correo electrónico o contraseña incorrectos.  2. Correo electrónico no encontrado en el sistema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. El correo electrónico es obligatorio.                     2. Por favor ingresa un correo electrónico válido. </t>
+  </si>
+  <si>
+    <t>1. La contraseña es obligatoria.                     2. Por favor ingrese más de 9 caracteres.</t>
   </si>
 </sst>
 </file>
@@ -535,11 +514,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA44"/>
+  <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -551,7 +530,7 @@
     <col min="9" max="9" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -592,64 +571,59 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" ht="39.6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="4">
-        <v>5</v>
-      </c>
-      <c r="O2" s="5">
-        <v>5</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="N2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -660,57 +634,54 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-    </row>
-    <row r="3" spans="1:27" ht="52.8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="I3" s="5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="5">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="O3" s="4">
-        <v>15</v>
-      </c>
-      <c r="P3" s="4">
-        <v>15</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -721,57 +692,54 @@
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-    </row>
-    <row r="4" spans="1:27" ht="52.8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:26" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="G4" s="5" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>20</v>
+        <v>39</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -782,57 +750,54 @@
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-    </row>
-    <row r="5" spans="1:27" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:26" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -843,57 +808,24 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-    </row>
-    <row r="6" spans="1:27" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>20</v>
-      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -904,9 +836,8 @@
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-    </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -922,7 +853,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -933,9 +864,8 @@
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -951,7 +881,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -962,9 +892,8 @@
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-    </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -980,7 +909,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -991,9 +920,8 @@
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1009,7 +937,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -1020,9 +948,8 @@
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1038,7 +965,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
@@ -1049,9 +976,8 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-    </row>
-    <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1067,7 +993,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -1078,9 +1004,8 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1096,7 +1021,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -1107,9 +1032,8 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1125,7 +1049,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
+      <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -1136,9 +1060,8 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1154,7 +1077,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -1165,9 +1088,8 @@
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-    </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1183,7 +1105,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -1194,9 +1116,8 @@
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-    </row>
-    <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1212,7 +1133,7 @@
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -1223,9 +1144,8 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-    </row>
-    <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1241,7 +1161,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
+      <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -1252,9 +1172,8 @@
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-    </row>
-    <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1270,7 +1189,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+      <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -1281,9 +1200,8 @@
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-    </row>
-    <row r="20" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1299,7 +1217,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+      <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -1310,9 +1228,8 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-    </row>
-    <row r="21" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1328,7 +1245,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
+      <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -1339,9 +1256,8 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-    </row>
-    <row r="22" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1357,7 +1273,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -1368,9 +1284,8 @@
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-    </row>
-    <row r="23" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1386,7 +1301,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
+      <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -1397,9 +1312,8 @@
       <c r="X23" s="1"/>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-    </row>
-    <row r="24" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1415,7 +1329,7 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
+      <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -1426,9 +1340,8 @@
       <c r="X24" s="1"/>
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-    </row>
-    <row r="25" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1444,7 +1357,7 @@
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
+      <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
@@ -1455,9 +1368,8 @@
       <c r="X25" s="1"/>
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-    </row>
-    <row r="26" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1473,7 +1385,7 @@
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
+      <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -1484,9 +1396,8 @@
       <c r="X26" s="1"/>
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
-      <c r="AA26" s="1"/>
-    </row>
-    <row r="27" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1502,7 +1413,7 @@
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
+      <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -1513,9 +1424,8 @@
       <c r="X27" s="1"/>
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
-      <c r="AA27" s="1"/>
-    </row>
-    <row r="28" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1531,7 +1441,7 @@
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -1542,9 +1452,8 @@
       <c r="X28" s="1"/>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
-    </row>
-    <row r="29" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1560,7 +1469,7 @@
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
+      <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
@@ -1571,9 +1480,8 @@
       <c r="X29" s="1"/>
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
-    </row>
-    <row r="30" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1589,7 +1497,7 @@
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
+      <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
@@ -1600,9 +1508,8 @@
       <c r="X30" s="1"/>
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
-      <c r="AA30" s="1"/>
-    </row>
-    <row r="31" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1618,7 +1525,7 @@
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
+      <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
@@ -1629,9 +1536,8 @@
       <c r="X31" s="1"/>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
-      <c r="AA31" s="1"/>
-    </row>
-    <row r="32" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1647,7 +1553,7 @@
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
+      <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -1658,9 +1564,8 @@
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
-      <c r="AA32" s="1"/>
-    </row>
-    <row r="33" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1676,7 +1581,7 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
+      <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -1687,9 +1592,8 @@
       <c r="X33" s="1"/>
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
-    </row>
-    <row r="34" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1705,7 +1609,7 @@
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
+      <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -1716,9 +1620,8 @@
       <c r="X34" s="1"/>
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
-      <c r="AA34" s="1"/>
-    </row>
-    <row r="35" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1734,7 +1637,7 @@
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
+      <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -1745,9 +1648,8 @@
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
-      <c r="AA35" s="1"/>
-    </row>
-    <row r="36" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1763,7 +1665,7 @@
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
+      <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -1774,9 +1676,8 @@
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
-      <c r="AA36" s="1"/>
-    </row>
-    <row r="37" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1792,7 +1693,7 @@
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
+      <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
@@ -1803,9 +1704,8 @@
       <c r="X37" s="1"/>
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
-      <c r="AA37" s="1"/>
-    </row>
-    <row r="38" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1821,7 +1721,7 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
+      <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
       <c r="S38" s="1"/>
@@ -1832,9 +1732,8 @@
       <c r="X38" s="1"/>
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
-      <c r="AA38" s="1"/>
-    </row>
-    <row r="39" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1850,7 +1749,7 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
+      <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
       <c r="S39" s="1"/>
@@ -1861,9 +1760,8 @@
       <c r="X39" s="1"/>
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
-      <c r="AA39" s="1"/>
-    </row>
-    <row r="40" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1879,7 +1777,7 @@
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
+      <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
@@ -1890,9 +1788,8 @@
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
-      <c r="AA40" s="1"/>
-    </row>
-    <row r="41" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1908,7 +1805,7 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
+      <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
@@ -1919,9 +1816,8 @@
       <c r="X41" s="1"/>
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
-      <c r="AA41" s="1"/>
-    </row>
-    <row r="42" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1937,7 +1833,7 @@
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
+      <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
@@ -1948,9 +1844,8 @@
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
-      <c r="AA42" s="1"/>
-    </row>
-    <row r="43" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1966,7 +1861,7 @@
       <c r="M43" s="2"/>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
+      <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
@@ -1977,36 +1872,6 @@
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
-      <c r="AA43" s="1"/>
-    </row>
-    <row r="44" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
-      <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
-      <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
-      <c r="Z44" s="1"/>
-      <c r="AA44" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>